<commit_message>
Made arcing shots more natural looking (8TbarNzz)
</commit_message>
<xml_diff>
--- a/Resources/Best Pass Parabola Formula.xlsx
+++ b/Resources/Best Pass Parabola Formula.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\Unity\Projects\unity-kings-of-the-beach\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A380922D-071E-4B78-BF5E-433ABF0FB18C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD2505F1-D8B4-4704-9ABA-38E16F301315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{AA972E6B-E75B-4653-8B65-AD33A2692674}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>t</t>
   </si>
@@ -55,18 +55,47 @@
   <si>
     <t>max</t>
   </si>
+  <si>
+    <t>Start-x</t>
+  </si>
+  <si>
+    <t>End-x</t>
+  </si>
+  <si>
+    <t>netCrossingT</t>
+  </si>
+  <si>
+    <t>heightAtNet</t>
+  </si>
+  <si>
+    <t>maxHeightPoint</t>
+  </si>
+  <si>
+    <t>requiredNetHeight</t>
+  </si>
+  <si>
+    <t>adjustedMaxHeight</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -92,9 +121,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -373,181 +404,181 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
-                  <c:v>3.2725333333333335</c:v>
+                  <c:v>3.6789777777777779</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.4181333333333335</c:v>
+                  <c:v>3.8499111111111111</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.5568</c:v>
+                  <c:v>4.0128000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.688533333333333</c:v>
+                  <c:v>4.1676444444444449</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.8133333333333335</c:v>
+                  <c:v>4.3144444444444447</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.9312</c:v>
+                  <c:v>4.4531999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.042133333333334</c:v>
+                  <c:v>4.583911111111111</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.1461333333333332</c:v>
+                  <c:v>4.7065777777777775</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.2431999999999999</c:v>
+                  <c:v>4.8212000000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.3333333333333339</c:v>
+                  <c:v>4.927777777777778</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.4165333333333336</c:v>
+                  <c:v>5.0263111111111112</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.4928000000000008</c:v>
+                  <c:v>5.1167999999999996</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.5621333333333336</c:v>
+                  <c:v>5.1992444444444441</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.6245333333333338</c:v>
+                  <c:v>5.2736444444444448</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4.68</c:v>
+                  <c:v>5.34</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.728533333333333</c:v>
+                  <c:v>5.3983111111111111</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.7701333333333338</c:v>
+                  <c:v>5.4485777777777784</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.8048000000000002</c:v>
+                  <c:v>5.4908000000000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.832533333333334</c:v>
+                  <c:v>5.524977777777778</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.8533333333333335</c:v>
+                  <c:v>5.5511111111111111</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.8672000000000004</c:v>
+                  <c:v>5.5692000000000004</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4.874133333333333</c:v>
+                  <c:v>5.579244444444444</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4.8741333333333339</c:v>
+                  <c:v>5.5812444444444447</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4.8672000000000004</c:v>
+                  <c:v>5.5752000000000006</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4.8533333333333335</c:v>
+                  <c:v>5.5611111111111109</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4.8325333333333331</c:v>
+                  <c:v>5.5389777777777782</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4.8048000000000002</c:v>
+                  <c:v>5.5087999999999999</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4.7701333333333338</c:v>
+                  <c:v>5.4705777777777778</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>4.728533333333333</c:v>
+                  <c:v>5.4243111111111109</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>4.68</c:v>
+                  <c:v>5.37</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>4.6245333333333338</c:v>
+                  <c:v>5.3076444444444437</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>4.5621333333333336</c:v>
+                  <c:v>5.2372444444444444</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>4.4927999999999999</c:v>
+                  <c:v>5.1587999999999994</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>4.4165333333333336</c:v>
+                  <c:v>5.0723111111111114</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>4.3333333333333339</c:v>
+                  <c:v>4.9777777777777779</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>4.2431999999999999</c:v>
+                  <c:v>4.8752000000000004</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4.1461333333333332</c:v>
+                  <c:v>4.7645777777777774</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4.042133333333334</c:v>
+                  <c:v>4.6459111111111113</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>3.9312</c:v>
+                  <c:v>4.5191999999999997</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>3.8133333333333339</c:v>
+                  <c:v>4.3844444444444441</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>3.6885333333333334</c:v>
+                  <c:v>4.2416444444444448</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>3.5568000000000004</c:v>
+                  <c:v>4.0908000000000007</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>3.4181333333333335</c:v>
+                  <c:v>3.9319111111111114</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>3.272533333333334</c:v>
+                  <c:v>3.7649777777777782</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>3.12</c:v>
+                  <c:v>3.59</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>2.9605333333333328</c:v>
+                  <c:v>3.4069777777777772</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>2.7941333333333334</c:v>
+                  <c:v>3.2159111111111112</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>2.6207999999999996</c:v>
+                  <c:v>3.0167999999999995</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>2.4405333333333337</c:v>
+                  <c:v>2.8096444444444444</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2.253333333333333</c:v>
+                  <c:v>2.5944444444444441</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>2.0592000000000006</c:v>
+                  <c:v>2.3712</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1.858133333333333</c:v>
+                  <c:v>2.1399111111111111</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>1.6501333333333339</c:v>
+                  <c:v>1.9005777777777781</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>1.4351999999999996</c:v>
+                  <c:v>1.6531999999999998</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>1.2133333333333338</c:v>
+                  <c:v>1.3977777777777787</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.98453333333333304</c:v>
+                  <c:v>1.1343111111111108</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.74880000000000069</c:v>
+                  <c:v>0.8628000000000009</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.50613333333333332</c:v>
+                  <c:v>0.58324444444444445</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.25653333333333406</c:v>
+                  <c:v>0.29564444444444543</c:v>
                 </c:pt>
                 <c:pt idx="59">
                   <c:v>0</c:v>
@@ -558,7 +589,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-DB75-4C18-BED1-729BF5B03605}"/>
+              <c16:uniqueId val="{00000000-96DE-4ABC-9403-52C1FA0A562E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -584,181 +615,181 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
-                  <c:v>3.1702666666666666</c:v>
+                  <c:v>3.5642555555555551</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.2170666666666667</c:v>
+                  <c:v>3.6243555555555553</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.2603999999999997</c:v>
+                  <c:v>3.6802999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.3002666666666669</c:v>
+                  <c:v>3.7320888888888888</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.3366666666666664</c:v>
+                  <c:v>3.779722222222222</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.3696000000000002</c:v>
+                  <c:v>3.8231999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.3990666666666667</c:v>
+                  <c:v>3.8625222222222222</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.4250666666666669</c:v>
+                  <c:v>3.8976888888888892</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.4476</c:v>
+                  <c:v>3.9286999999999996</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.4666666666666668</c:v>
+                  <c:v>3.9555555555555557</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.4822666666666664</c:v>
+                  <c:v>3.9782555555555552</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.4944000000000006</c:v>
+                  <c:v>3.9968000000000004</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.5030666666666663</c:v>
+                  <c:v>4.0111888888888885</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.5082666666666662</c:v>
+                  <c:v>4.0214222222222222</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.51</c:v>
+                  <c:v>4.0274999999999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.5082666666666671</c:v>
+                  <c:v>4.0294222222222231</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.5030666666666663</c:v>
+                  <c:v>4.0271888888888894</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.4943999999999997</c:v>
+                  <c:v>4.0207999999999995</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.4822666666666668</c:v>
+                  <c:v>4.0102555555555552</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.4666666666666668</c:v>
+                  <c:v>3.9955555555555562</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.4475999999999996</c:v>
+                  <c:v>3.9767000000000001</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3.425066666666666</c:v>
+                  <c:v>3.9536888888888884</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3.3990666666666671</c:v>
+                  <c:v>3.9265222222222231</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.3696000000000002</c:v>
+                  <c:v>3.8952</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.336666666666666</c:v>
+                  <c:v>3.8597222222222216</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.3002666666666665</c:v>
+                  <c:v>3.8200888888888889</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3.2604000000000006</c:v>
+                  <c:v>3.7763000000000009</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>3.2170666666666663</c:v>
+                  <c:v>3.7283555555555559</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>3.1702666666666661</c:v>
+                  <c:v>3.6762555555555556</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3.12</c:v>
+                  <c:v>3.62</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3.0662666666666665</c:v>
+                  <c:v>3.5595888888888889</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.0090666666666666</c:v>
+                  <c:v>3.4950222222222225</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.9483999999999995</c:v>
+                  <c:v>3.4262999999999999</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.884266666666667</c:v>
+                  <c:v>3.3534222222222225</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.8166666666666664</c:v>
+                  <c:v>3.276388888888889</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.7456</c:v>
+                  <c:v>3.1952000000000003</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2.6710666666666665</c:v>
+                  <c:v>3.1098555555555554</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2.5930666666666666</c:v>
+                  <c:v>3.0203555555555557</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2.5115999999999996</c:v>
+                  <c:v>2.9266999999999999</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2.4266666666666667</c:v>
+                  <c:v>2.8288888888888892</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2.3382666666666667</c:v>
+                  <c:v>2.726922222222222</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2.2464</c:v>
+                  <c:v>2.6208000000000005</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>2.1510666666666665</c:v>
+                  <c:v>2.5105222222222223</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2.0522666666666671</c:v>
+                  <c:v>2.3960888888888898</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1.95</c:v>
+                  <c:v>2.2774999999999999</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1.8442666666666663</c:v>
+                  <c:v>2.1547555555555555</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1.7350666666666665</c:v>
+                  <c:v>2.0278555555555555</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1.6223999999999996</c:v>
+                  <c:v>1.8967999999999996</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1.5062666666666666</c:v>
+                  <c:v>1.7615888888888891</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1.3866666666666665</c:v>
+                  <c:v>1.622222222222222</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1.2636000000000001</c:v>
+                  <c:v>1.4787000000000001</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1.1370666666666662</c:v>
+                  <c:v>1.3310222222222221</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>1.0070666666666668</c:v>
+                  <c:v>1.1791888888888893</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.87359999999999982</c:v>
+                  <c:v>1.0231999999999999</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.73666666666666702</c:v>
+                  <c:v>0.86305555555555602</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.5962666666666665</c:v>
+                  <c:v>0.69875555555555535</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.45240000000000041</c:v>
+                  <c:v>0.53030000000000055</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.3050666666666666</c:v>
+                  <c:v>0.35768888888888883</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.15426666666666713</c:v>
+                  <c:v>0.18092222222222279</c:v>
                 </c:pt>
                 <c:pt idx="59">
                   <c:v>0</c:v>
@@ -769,7 +800,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-DB75-4C18-BED1-729BF5B03605}"/>
+              <c16:uniqueId val="{00000001-96DE-4ABC-9403-52C1FA0A562E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1505,22 +1536,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>32657</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>48986</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>32657</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>16329</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8245D367-3808-4AB8-B0E8-4781DCB6AF2E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9886004D-2BD9-47AF-9456-1224F6EE2ECB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1867,6 +1898,10 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="7" max="7" width="1.69140625" customWidth="1"/>
+    <col min="8" max="8" width="16.53515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
@@ -1890,29 +1925,29 @@
         <f>(ROW()-1)/60</f>
         <v>1.6666666666666666E-2</v>
       </c>
-      <c r="B2">
-        <v>3.12</v>
+      <c r="B2" s="2">
+        <v>3.5</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2">
-        <v>3.12</v>
+      <c r="D2" s="2">
+        <v>3.62</v>
       </c>
       <c r="E2" s="1">
         <f>4*D2*A2*(1-A2)+(B2+(C2-B2)*A2)</f>
-        <v>3.2725333333333335</v>
+        <v>3.6789777777777779</v>
       </c>
       <c r="F2">
         <f>(1-A2)*(1-A2)*B2+2*(1-A2)*A2*((D2-0.25*B2-0.25*C2)/0.5)+A2*A2*C2</f>
-        <v>3.1702666666666666</v>
+        <v>3.5642555555555551</v>
       </c>
       <c r="H2" t="s">
         <v>1</v>
       </c>
       <c r="I2">
         <f>F2</f>
-        <v>3.1702666666666666</v>
+        <v>3.5642555555555551</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.4">
@@ -1922,7 +1957,7 @@
       </c>
       <c r="B3">
         <f>B2</f>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:D18" si="1">C2</f>
@@ -1930,22 +1965,22 @@
       </c>
       <c r="D3">
         <f t="shared" si="1"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E61" si="2">4*D3*A3*(1-A3)+(B3+(C3-B3)*A3)</f>
-        <v>3.4181333333333335</v>
+        <v>3.8499111111111111</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F61" si="3">(1-A3)*(1-A3)*B3+2*(1-A3)*A3*((D3-0.25*B3-0.25*C3)/0.5)+A3*A3*C3</f>
-        <v>3.2170666666666667</v>
+        <v>3.6243555555555553</v>
       </c>
       <c r="H3" t="s">
         <v>5</v>
       </c>
       <c r="I3">
         <f>MAX(F:F)</f>
-        <v>3.51</v>
+        <v>4.0294222222222231</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.4">
@@ -1955,7 +1990,7 @@
       </c>
       <c r="B4">
         <f t="shared" ref="B4:B61" si="4">B3</f>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C4">
         <f t="shared" si="1"/>
@@ -1963,15 +1998,15 @@
       </c>
       <c r="D4">
         <f t="shared" si="1"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" si="2"/>
-        <v>3.5568</v>
+        <v>4.0128000000000004</v>
       </c>
       <c r="F4">
         <f t="shared" si="3"/>
-        <v>3.2603999999999997</v>
+        <v>3.6802999999999999</v>
       </c>
       <c r="H4" t="s">
         <v>2</v>
@@ -1988,7 +2023,7 @@
       </c>
       <c r="B5">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
@@ -1996,15 +2031,15 @@
       </c>
       <c r="D5">
         <f t="shared" si="1"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" si="2"/>
-        <v>3.688533333333333</v>
+        <v>4.1676444444444449</v>
       </c>
       <c r="F5">
         <f t="shared" si="3"/>
-        <v>3.3002666666666669</v>
+        <v>3.7320888888888888</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.4">
@@ -2014,7 +2049,7 @@
       </c>
       <c r="B6">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
@@ -2022,15 +2057,21 @@
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="2"/>
-        <v>3.8133333333333335</v>
+        <v>4.3144444444444447</v>
       </c>
       <c r="F6">
         <f t="shared" si="3"/>
-        <v>3.3366666666666664</v>
+        <v>3.779722222222222</v>
+      </c>
+      <c r="H6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="2">
+        <v>-3.5</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.4">
@@ -2040,7 +2081,7 @@
       </c>
       <c r="B7">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
@@ -2048,15 +2089,21 @@
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" si="2"/>
-        <v>3.9312</v>
+        <v>4.4531999999999998</v>
       </c>
       <c r="F7">
         <f t="shared" si="3"/>
-        <v>3.3696000000000002</v>
+        <v>3.8231999999999999</v>
+      </c>
+      <c r="H7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="2">
+        <v>6.78</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.4">
@@ -2066,7 +2113,7 @@
       </c>
       <c r="B8">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
@@ -2074,15 +2121,22 @@
       </c>
       <c r="D8">
         <f t="shared" si="1"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="2"/>
-        <v>4.042133333333334</v>
+        <v>4.583911111111111</v>
       </c>
       <c r="F8">
         <f t="shared" si="3"/>
-        <v>3.3990666666666667</v>
+        <v>3.8625222222222222</v>
+      </c>
+      <c r="H8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="1">
+        <f>ABS(I6)/ABS(I7-I6)</f>
+        <v>0.34046692607003887</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.4">
@@ -2092,7 +2146,7 @@
       </c>
       <c r="B9">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
@@ -2100,15 +2154,15 @@
       </c>
       <c r="D9">
         <f t="shared" si="1"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="2"/>
-        <v>4.1461333333333332</v>
+        <v>4.7065777777777775</v>
       </c>
       <c r="F9">
         <f t="shared" si="3"/>
-        <v>3.4250666666666669</v>
+        <v>3.8976888888888892</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.4">
@@ -2118,7 +2172,7 @@
       </c>
       <c r="B10">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
@@ -2126,15 +2180,22 @@
       </c>
       <c r="D10">
         <f t="shared" si="1"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="2"/>
-        <v>4.2431999999999999</v>
+        <v>4.8212000000000002</v>
       </c>
       <c r="F10">
         <f t="shared" si="3"/>
-        <v>3.4476</v>
+        <v>3.9286999999999996</v>
+      </c>
+      <c r="H10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" s="3">
+        <f>(1-I8)*(1-I8)*B2+2*(1-I8)*I8*((D2-0.25*B2-0.25*C2)/0.5)+I8*I8*C2</f>
+        <v>3.9879937622068473</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.4">
@@ -2144,7 +2205,7 @@
       </c>
       <c r="B11">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
@@ -2152,15 +2213,22 @@
       </c>
       <c r="D11">
         <f t="shared" si="1"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="2"/>
-        <v>4.3333333333333339</v>
+        <v>4.927777777777778</v>
       </c>
       <c r="F11">
         <f t="shared" si="3"/>
-        <v>3.4666666666666668</v>
+        <v>3.9555555555555557</v>
+      </c>
+      <c r="H11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11">
+        <f>D2</f>
+        <v>3.62</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
@@ -2170,7 +2238,7 @@
       </c>
       <c r="B12">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
@@ -2178,15 +2246,21 @@
       </c>
       <c r="D12">
         <f t="shared" si="1"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="2"/>
-        <v>4.4165333333333336</v>
+        <v>5.0263111111111112</v>
       </c>
       <c r="F12">
         <f t="shared" si="3"/>
-        <v>3.4822666666666664</v>
+        <v>3.9782555555555552</v>
+      </c>
+      <c r="H12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="2">
+        <v>2.5</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.4">
@@ -2196,7 +2270,7 @@
       </c>
       <c r="B13">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
@@ -2204,15 +2278,22 @@
       </c>
       <c r="D13">
         <f t="shared" si="1"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="2"/>
-        <v>4.4928000000000008</v>
+        <v>5.1167999999999996</v>
       </c>
       <c r="F13">
         <f t="shared" si="3"/>
-        <v>3.4944000000000006</v>
+        <v>3.9968000000000004</v>
+      </c>
+      <c r="H13" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13" s="3">
+        <f>I11+I12-I10</f>
+        <v>2.1320062377931528</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.4">
@@ -2222,7 +2303,7 @@
       </c>
       <c r="B14">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
@@ -2230,15 +2311,15 @@
       </c>
       <c r="D14">
         <f t="shared" si="1"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" si="2"/>
-        <v>4.5621333333333336</v>
+        <v>5.1992444444444441</v>
       </c>
       <c r="F14">
         <f t="shared" si="3"/>
-        <v>3.5030666666666663</v>
+        <v>4.0111888888888885</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">
@@ -2248,7 +2329,7 @@
       </c>
       <c r="B15">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
@@ -2256,15 +2337,15 @@
       </c>
       <c r="D15">
         <f t="shared" si="1"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" si="2"/>
-        <v>4.6245333333333338</v>
+        <v>5.2736444444444448</v>
       </c>
       <c r="F15">
         <f t="shared" si="3"/>
-        <v>3.5082666666666662</v>
+        <v>4.0214222222222222</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.4">
@@ -2274,7 +2355,7 @@
       </c>
       <c r="B16">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
@@ -2282,15 +2363,15 @@
       </c>
       <c r="D16">
         <f t="shared" si="1"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E16" s="1">
         <f t="shared" si="2"/>
-        <v>4.68</v>
+        <v>5.34</v>
       </c>
       <c r="F16">
         <f t="shared" si="3"/>
-        <v>3.51</v>
+        <v>4.0274999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.4">
@@ -2300,7 +2381,7 @@
       </c>
       <c r="B17">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
@@ -2308,15 +2389,15 @@
       </c>
       <c r="D17">
         <f t="shared" si="1"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E17" s="1">
         <f t="shared" si="2"/>
-        <v>4.728533333333333</v>
+        <v>5.3983111111111111</v>
       </c>
       <c r="F17">
         <f t="shared" si="3"/>
-        <v>3.5082666666666671</v>
+        <v>4.0294222222222231</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.4">
@@ -2326,7 +2407,7 @@
       </c>
       <c r="B18">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C18">
         <f t="shared" si="1"/>
@@ -2334,15 +2415,15 @@
       </c>
       <c r="D18">
         <f t="shared" si="1"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E18" s="1">
         <f t="shared" si="2"/>
-        <v>4.7701333333333338</v>
+        <v>5.4485777777777784</v>
       </c>
       <c r="F18">
         <f t="shared" si="3"/>
-        <v>3.5030666666666663</v>
+        <v>4.0271888888888894</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.4">
@@ -2352,7 +2433,7 @@
       </c>
       <c r="B19">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C19">
         <f t="shared" ref="C19:C61" si="5">C18</f>
@@ -2360,15 +2441,15 @@
       </c>
       <c r="D19">
         <f t="shared" ref="D19:D61" si="6">D18</f>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E19" s="1">
         <f t="shared" si="2"/>
-        <v>4.8048000000000002</v>
+        <v>5.4908000000000001</v>
       </c>
       <c r="F19">
         <f t="shared" si="3"/>
-        <v>3.4943999999999997</v>
+        <v>4.0207999999999995</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.4">
@@ -2378,7 +2459,7 @@
       </c>
       <c r="B20">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C20">
         <f t="shared" si="5"/>
@@ -2386,15 +2467,15 @@
       </c>
       <c r="D20">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E20" s="1">
         <f t="shared" si="2"/>
-        <v>4.832533333333334</v>
+        <v>5.524977777777778</v>
       </c>
       <c r="F20">
         <f t="shared" si="3"/>
-        <v>3.4822666666666668</v>
+        <v>4.0102555555555552</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.4">
@@ -2404,7 +2485,7 @@
       </c>
       <c r="B21">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C21">
         <f t="shared" si="5"/>
@@ -2412,15 +2493,15 @@
       </c>
       <c r="D21">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E21" s="1">
         <f t="shared" si="2"/>
-        <v>4.8533333333333335</v>
+        <v>5.5511111111111111</v>
       </c>
       <c r="F21">
         <f t="shared" si="3"/>
-        <v>3.4666666666666668</v>
+        <v>3.9955555555555562</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.4">
@@ -2430,7 +2511,7 @@
       </c>
       <c r="B22">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C22">
         <f t="shared" si="5"/>
@@ -2438,15 +2519,15 @@
       </c>
       <c r="D22">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E22" s="1">
         <f t="shared" si="2"/>
-        <v>4.8672000000000004</v>
+        <v>5.5692000000000004</v>
       </c>
       <c r="F22">
         <f t="shared" si="3"/>
-        <v>3.4475999999999996</v>
+        <v>3.9767000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.4">
@@ -2456,7 +2537,7 @@
       </c>
       <c r="B23">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C23">
         <f t="shared" si="5"/>
@@ -2464,15 +2545,15 @@
       </c>
       <c r="D23">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E23" s="1">
         <f t="shared" si="2"/>
-        <v>4.874133333333333</v>
+        <v>5.579244444444444</v>
       </c>
       <c r="F23">
         <f t="shared" si="3"/>
-        <v>3.425066666666666</v>
+        <v>3.9536888888888884</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.4">
@@ -2482,7 +2563,7 @@
       </c>
       <c r="B24">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C24">
         <f t="shared" si="5"/>
@@ -2490,15 +2571,15 @@
       </c>
       <c r="D24">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E24" s="1">
         <f t="shared" si="2"/>
-        <v>4.8741333333333339</v>
+        <v>5.5812444444444447</v>
       </c>
       <c r="F24">
         <f t="shared" si="3"/>
-        <v>3.3990666666666671</v>
+        <v>3.9265222222222231</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.4">
@@ -2508,7 +2589,7 @@
       </c>
       <c r="B25">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C25">
         <f t="shared" si="5"/>
@@ -2516,15 +2597,15 @@
       </c>
       <c r="D25">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E25" s="1">
         <f t="shared" si="2"/>
-        <v>4.8672000000000004</v>
+        <v>5.5752000000000006</v>
       </c>
       <c r="F25">
         <f t="shared" si="3"/>
-        <v>3.3696000000000002</v>
+        <v>3.8952</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.4">
@@ -2534,7 +2615,7 @@
       </c>
       <c r="B26">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C26">
         <f t="shared" si="5"/>
@@ -2542,15 +2623,15 @@
       </c>
       <c r="D26">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E26" s="1">
         <f t="shared" si="2"/>
-        <v>4.8533333333333335</v>
+        <v>5.5611111111111109</v>
       </c>
       <c r="F26">
         <f t="shared" si="3"/>
-        <v>3.336666666666666</v>
+        <v>3.8597222222222216</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.4">
@@ -2560,7 +2641,7 @@
       </c>
       <c r="B27">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C27">
         <f t="shared" si="5"/>
@@ -2568,15 +2649,15 @@
       </c>
       <c r="D27">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E27" s="1">
         <f t="shared" si="2"/>
-        <v>4.8325333333333331</v>
+        <v>5.5389777777777782</v>
       </c>
       <c r="F27">
         <f t="shared" si="3"/>
-        <v>3.3002666666666665</v>
+        <v>3.8200888888888889</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.4">
@@ -2586,7 +2667,7 @@
       </c>
       <c r="B28">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C28">
         <f t="shared" si="5"/>
@@ -2594,15 +2675,15 @@
       </c>
       <c r="D28">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E28" s="1">
         <f t="shared" si="2"/>
-        <v>4.8048000000000002</v>
+        <v>5.5087999999999999</v>
       </c>
       <c r="F28">
         <f t="shared" si="3"/>
-        <v>3.2604000000000006</v>
+        <v>3.7763000000000009</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.4">
@@ -2612,7 +2693,7 @@
       </c>
       <c r="B29">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C29">
         <f t="shared" si="5"/>
@@ -2620,15 +2701,15 @@
       </c>
       <c r="D29">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E29" s="1">
         <f t="shared" si="2"/>
-        <v>4.7701333333333338</v>
+        <v>5.4705777777777778</v>
       </c>
       <c r="F29">
         <f t="shared" si="3"/>
-        <v>3.2170666666666663</v>
+        <v>3.7283555555555559</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.4">
@@ -2638,7 +2719,7 @@
       </c>
       <c r="B30">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C30">
         <f t="shared" si="5"/>
@@ -2646,15 +2727,15 @@
       </c>
       <c r="D30">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E30" s="1">
         <f t="shared" si="2"/>
-        <v>4.728533333333333</v>
+        <v>5.4243111111111109</v>
       </c>
       <c r="F30">
         <f t="shared" si="3"/>
-        <v>3.1702666666666661</v>
+        <v>3.6762555555555556</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.4">
@@ -2664,7 +2745,7 @@
       </c>
       <c r="B31">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C31">
         <f t="shared" si="5"/>
@@ -2672,15 +2753,15 @@
       </c>
       <c r="D31">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E31" s="1">
         <f t="shared" si="2"/>
-        <v>4.68</v>
+        <v>5.37</v>
       </c>
       <c r="F31">
         <f t="shared" si="3"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.4">
@@ -2690,7 +2771,7 @@
       </c>
       <c r="B32">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C32">
         <f t="shared" si="5"/>
@@ -2698,15 +2779,15 @@
       </c>
       <c r="D32">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E32" s="1">
         <f t="shared" si="2"/>
-        <v>4.6245333333333338</v>
+        <v>5.3076444444444437</v>
       </c>
       <c r="F32">
         <f t="shared" si="3"/>
-        <v>3.0662666666666665</v>
+        <v>3.5595888888888889</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.4">
@@ -2716,7 +2797,7 @@
       </c>
       <c r="B33">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C33">
         <f t="shared" si="5"/>
@@ -2724,15 +2805,15 @@
       </c>
       <c r="D33">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E33" s="1">
         <f t="shared" si="2"/>
-        <v>4.5621333333333336</v>
+        <v>5.2372444444444444</v>
       </c>
       <c r="F33">
         <f t="shared" si="3"/>
-        <v>3.0090666666666666</v>
+        <v>3.4950222222222225</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.4">
@@ -2742,7 +2823,7 @@
       </c>
       <c r="B34">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C34">
         <f t="shared" si="5"/>
@@ -2750,15 +2831,15 @@
       </c>
       <c r="D34">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E34" s="1">
         <f t="shared" si="2"/>
-        <v>4.4927999999999999</v>
+        <v>5.1587999999999994</v>
       </c>
       <c r="F34">
         <f t="shared" si="3"/>
-        <v>2.9483999999999995</v>
+        <v>3.4262999999999999</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.4">
@@ -2768,7 +2849,7 @@
       </c>
       <c r="B35">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C35">
         <f t="shared" si="5"/>
@@ -2776,15 +2857,15 @@
       </c>
       <c r="D35">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E35" s="1">
         <f t="shared" si="2"/>
-        <v>4.4165333333333336</v>
+        <v>5.0723111111111114</v>
       </c>
       <c r="F35">
         <f t="shared" si="3"/>
-        <v>2.884266666666667</v>
+        <v>3.3534222222222225</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.4">
@@ -2794,7 +2875,7 @@
       </c>
       <c r="B36">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C36">
         <f t="shared" si="5"/>
@@ -2802,15 +2883,15 @@
       </c>
       <c r="D36">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E36" s="1">
         <f t="shared" si="2"/>
-        <v>4.3333333333333339</v>
+        <v>4.9777777777777779</v>
       </c>
       <c r="F36">
         <f t="shared" si="3"/>
-        <v>2.8166666666666664</v>
+        <v>3.276388888888889</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.4">
@@ -2820,7 +2901,7 @@
       </c>
       <c r="B37">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C37">
         <f t="shared" si="5"/>
@@ -2828,15 +2909,15 @@
       </c>
       <c r="D37">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E37" s="1">
         <f t="shared" si="2"/>
-        <v>4.2431999999999999</v>
+        <v>4.8752000000000004</v>
       </c>
       <c r="F37">
         <f t="shared" si="3"/>
-        <v>2.7456</v>
+        <v>3.1952000000000003</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.4">
@@ -2846,7 +2927,7 @@
       </c>
       <c r="B38">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C38">
         <f t="shared" si="5"/>
@@ -2854,15 +2935,15 @@
       </c>
       <c r="D38">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E38" s="1">
         <f t="shared" si="2"/>
-        <v>4.1461333333333332</v>
+        <v>4.7645777777777774</v>
       </c>
       <c r="F38">
         <f t="shared" si="3"/>
-        <v>2.6710666666666665</v>
+        <v>3.1098555555555554</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.4">
@@ -2872,7 +2953,7 @@
       </c>
       <c r="B39">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C39">
         <f t="shared" si="5"/>
@@ -2880,15 +2961,15 @@
       </c>
       <c r="D39">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E39" s="1">
         <f t="shared" si="2"/>
-        <v>4.042133333333334</v>
+        <v>4.6459111111111113</v>
       </c>
       <c r="F39">
         <f t="shared" si="3"/>
-        <v>2.5930666666666666</v>
+        <v>3.0203555555555557</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.4">
@@ -2898,7 +2979,7 @@
       </c>
       <c r="B40">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C40">
         <f t="shared" si="5"/>
@@ -2906,15 +2987,15 @@
       </c>
       <c r="D40">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E40" s="1">
         <f t="shared" si="2"/>
-        <v>3.9312</v>
+        <v>4.5191999999999997</v>
       </c>
       <c r="F40">
         <f t="shared" si="3"/>
-        <v>2.5115999999999996</v>
+        <v>2.9266999999999999</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.4">
@@ -2924,7 +3005,7 @@
       </c>
       <c r="B41">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C41">
         <f t="shared" si="5"/>
@@ -2932,15 +3013,15 @@
       </c>
       <c r="D41">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E41" s="1">
         <f t="shared" si="2"/>
-        <v>3.8133333333333339</v>
+        <v>4.3844444444444441</v>
       </c>
       <c r="F41">
         <f t="shared" si="3"/>
-        <v>2.4266666666666667</v>
+        <v>2.8288888888888892</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.4">
@@ -2950,7 +3031,7 @@
       </c>
       <c r="B42">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C42">
         <f t="shared" si="5"/>
@@ -2958,15 +3039,15 @@
       </c>
       <c r="D42">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E42" s="1">
         <f t="shared" si="2"/>
-        <v>3.6885333333333334</v>
+        <v>4.2416444444444448</v>
       </c>
       <c r="F42">
         <f t="shared" si="3"/>
-        <v>2.3382666666666667</v>
+        <v>2.726922222222222</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.4">
@@ -2976,7 +3057,7 @@
       </c>
       <c r="B43">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C43">
         <f t="shared" si="5"/>
@@ -2984,15 +3065,15 @@
       </c>
       <c r="D43">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E43" s="1">
         <f t="shared" si="2"/>
-        <v>3.5568000000000004</v>
+        <v>4.0908000000000007</v>
       </c>
       <c r="F43">
         <f t="shared" si="3"/>
-        <v>2.2464</v>
+        <v>2.6208000000000005</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.4">
@@ -3002,7 +3083,7 @@
       </c>
       <c r="B44">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C44">
         <f t="shared" si="5"/>
@@ -3010,15 +3091,15 @@
       </c>
       <c r="D44">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E44" s="1">
         <f t="shared" si="2"/>
-        <v>3.4181333333333335</v>
+        <v>3.9319111111111114</v>
       </c>
       <c r="F44">
         <f t="shared" si="3"/>
-        <v>2.1510666666666665</v>
+        <v>2.5105222222222223</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.4">
@@ -3028,7 +3109,7 @@
       </c>
       <c r="B45">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C45">
         <f t="shared" si="5"/>
@@ -3036,15 +3117,15 @@
       </c>
       <c r="D45">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E45" s="1">
         <f t="shared" si="2"/>
-        <v>3.272533333333334</v>
+        <v>3.7649777777777782</v>
       </c>
       <c r="F45">
         <f t="shared" si="3"/>
-        <v>2.0522666666666671</v>
+        <v>2.3960888888888898</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.4">
@@ -3054,7 +3135,7 @@
       </c>
       <c r="B46">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C46">
         <f t="shared" si="5"/>
@@ -3062,15 +3143,15 @@
       </c>
       <c r="D46">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E46" s="1">
         <f t="shared" si="2"/>
-        <v>3.12</v>
+        <v>3.59</v>
       </c>
       <c r="F46">
         <f t="shared" si="3"/>
-        <v>1.95</v>
+        <v>2.2774999999999999</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.4">
@@ -3080,7 +3161,7 @@
       </c>
       <c r="B47">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C47">
         <f t="shared" si="5"/>
@@ -3088,15 +3169,15 @@
       </c>
       <c r="D47">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E47" s="1">
         <f t="shared" si="2"/>
-        <v>2.9605333333333328</v>
+        <v>3.4069777777777772</v>
       </c>
       <c r="F47">
         <f t="shared" si="3"/>
-        <v>1.8442666666666663</v>
+        <v>2.1547555555555555</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.4">
@@ -3106,7 +3187,7 @@
       </c>
       <c r="B48">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C48">
         <f t="shared" si="5"/>
@@ -3114,15 +3195,15 @@
       </c>
       <c r="D48">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E48" s="1">
         <f t="shared" si="2"/>
-        <v>2.7941333333333334</v>
+        <v>3.2159111111111112</v>
       </c>
       <c r="F48">
         <f t="shared" si="3"/>
-        <v>1.7350666666666665</v>
+        <v>2.0278555555555555</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.4">
@@ -3132,7 +3213,7 @@
       </c>
       <c r="B49">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C49">
         <f t="shared" si="5"/>
@@ -3140,15 +3221,15 @@
       </c>
       <c r="D49">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E49" s="1">
         <f t="shared" si="2"/>
-        <v>2.6207999999999996</v>
+        <v>3.0167999999999995</v>
       </c>
       <c r="F49">
         <f t="shared" si="3"/>
-        <v>1.6223999999999996</v>
+        <v>1.8967999999999996</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.4">
@@ -3158,7 +3239,7 @@
       </c>
       <c r="B50">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C50">
         <f t="shared" si="5"/>
@@ -3166,15 +3247,15 @@
       </c>
       <c r="D50">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E50" s="1">
         <f t="shared" si="2"/>
-        <v>2.4405333333333337</v>
+        <v>2.8096444444444444</v>
       </c>
       <c r="F50">
         <f t="shared" si="3"/>
-        <v>1.5062666666666666</v>
+        <v>1.7615888888888891</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.4">
@@ -3184,7 +3265,7 @@
       </c>
       <c r="B51">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C51">
         <f t="shared" si="5"/>
@@ -3192,15 +3273,15 @@
       </c>
       <c r="D51">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E51" s="1">
         <f t="shared" si="2"/>
-        <v>2.253333333333333</v>
+        <v>2.5944444444444441</v>
       </c>
       <c r="F51">
         <f t="shared" si="3"/>
-        <v>1.3866666666666665</v>
+        <v>1.622222222222222</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.4">
@@ -3210,7 +3291,7 @@
       </c>
       <c r="B52">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C52">
         <f t="shared" si="5"/>
@@ -3218,15 +3299,15 @@
       </c>
       <c r="D52">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E52" s="1">
         <f t="shared" si="2"/>
-        <v>2.0592000000000006</v>
+        <v>2.3712</v>
       </c>
       <c r="F52">
         <f t="shared" si="3"/>
-        <v>1.2636000000000001</v>
+        <v>1.4787000000000001</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.4">
@@ -3236,7 +3317,7 @@
       </c>
       <c r="B53">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C53">
         <f t="shared" si="5"/>
@@ -3244,15 +3325,15 @@
       </c>
       <c r="D53">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E53" s="1">
         <f t="shared" si="2"/>
-        <v>1.858133333333333</v>
+        <v>2.1399111111111111</v>
       </c>
       <c r="F53">
         <f t="shared" si="3"/>
-        <v>1.1370666666666662</v>
+        <v>1.3310222222222221</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.4">
@@ -3262,7 +3343,7 @@
       </c>
       <c r="B54">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C54">
         <f t="shared" si="5"/>
@@ -3270,15 +3351,15 @@
       </c>
       <c r="D54">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E54" s="1">
         <f t="shared" si="2"/>
-        <v>1.6501333333333339</v>
+        <v>1.9005777777777781</v>
       </c>
       <c r="F54">
         <f t="shared" si="3"/>
-        <v>1.0070666666666668</v>
+        <v>1.1791888888888893</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.4">
@@ -3288,7 +3369,7 @@
       </c>
       <c r="B55">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C55">
         <f t="shared" si="5"/>
@@ -3296,15 +3377,15 @@
       </c>
       <c r="D55">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E55" s="1">
         <f t="shared" si="2"/>
-        <v>1.4351999999999996</v>
+        <v>1.6531999999999998</v>
       </c>
       <c r="F55">
         <f t="shared" si="3"/>
-        <v>0.87359999999999982</v>
+        <v>1.0231999999999999</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.4">
@@ -3314,7 +3395,7 @@
       </c>
       <c r="B56">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C56">
         <f t="shared" si="5"/>
@@ -3322,15 +3403,15 @@
       </c>
       <c r="D56">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E56" s="1">
         <f t="shared" si="2"/>
-        <v>1.2133333333333338</v>
+        <v>1.3977777777777787</v>
       </c>
       <c r="F56">
         <f t="shared" si="3"/>
-        <v>0.73666666666666702</v>
+        <v>0.86305555555555602</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.4">
@@ -3340,7 +3421,7 @@
       </c>
       <c r="B57">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C57">
         <f t="shared" si="5"/>
@@ -3348,15 +3429,15 @@
       </c>
       <c r="D57">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E57" s="1">
         <f t="shared" si="2"/>
-        <v>0.98453333333333304</v>
+        <v>1.1343111111111108</v>
       </c>
       <c r="F57">
         <f t="shared" si="3"/>
-        <v>0.5962666666666665</v>
+        <v>0.69875555555555535</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.4">
@@ -3366,7 +3447,7 @@
       </c>
       <c r="B58">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C58">
         <f t="shared" si="5"/>
@@ -3374,15 +3455,15 @@
       </c>
       <c r="D58">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E58" s="1">
         <f t="shared" si="2"/>
-        <v>0.74880000000000069</v>
+        <v>0.8628000000000009</v>
       </c>
       <c r="F58">
         <f t="shared" si="3"/>
-        <v>0.45240000000000041</v>
+        <v>0.53030000000000055</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.4">
@@ -3392,7 +3473,7 @@
       </c>
       <c r="B59">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C59">
         <f t="shared" si="5"/>
@@ -3400,15 +3481,15 @@
       </c>
       <c r="D59">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E59" s="1">
         <f t="shared" si="2"/>
-        <v>0.50613333333333332</v>
+        <v>0.58324444444444445</v>
       </c>
       <c r="F59">
         <f t="shared" si="3"/>
-        <v>0.3050666666666666</v>
+        <v>0.35768888888888883</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.4">
@@ -3418,7 +3499,7 @@
       </c>
       <c r="B60">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C60">
         <f t="shared" si="5"/>
@@ -3426,15 +3507,15 @@
       </c>
       <c r="D60">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E60" s="1">
         <f t="shared" si="2"/>
-        <v>0.25653333333333406</v>
+        <v>0.29564444444444543</v>
       </c>
       <c r="F60">
         <f t="shared" si="3"/>
-        <v>0.15426666666666713</v>
+        <v>0.18092222222222279</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.4">
@@ -3444,7 +3525,7 @@
       </c>
       <c r="B61">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>3.5</v>
       </c>
       <c r="C61">
         <f t="shared" si="5"/>
@@ -3452,7 +3533,7 @@
       </c>
       <c r="D61">
         <f t="shared" si="6"/>
-        <v>3.12</v>
+        <v>3.62</v>
       </c>
       <c r="E61" s="1">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
Attempt to fix blocking in to net (ZK3DXh7P)
</commit_message>
<xml_diff>
--- a/Resources/Best Pass Parabola Formula.xlsx
+++ b/Resources/Best Pass Parabola Formula.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\Unity\Projects\unity-kings-of-the-beach\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD2505F1-D8B4-4704-9ABA-38E16F301315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0029A0-C45D-492D-BDFF-2B3BCA21B054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{AA972E6B-E75B-4653-8B65-AD33A2692674}"/>
+    <workbookView xWindow="3540" yWindow="1260" windowWidth="24034" windowHeight="10894" xr2:uid="{AA972E6B-E75B-4653-8B65-AD33A2692674}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -84,7 +84,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +96,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF00B0F0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -121,11 +128,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -190,6 +199,230 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$61</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>5.2211864888888879</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1FAC-412F-950E-94BC68936225}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="100060928"/>
+        <c:axId val="375890064"/>
+      </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -404,181 +637,181 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
-                  <c:v>3.6789777777777779</c:v>
+                  <c:v>3.6979761055555556</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.8499111111111111</c:v>
+                  <c:v>3.8416738222222224</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0128000000000004</c:v>
+                  <c:v>3.9782551499999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.1676444444444449</c:v>
+                  <c:v>4.1077200888888896</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.3144444444444447</c:v>
+                  <c:v>4.2300686388888886</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.4531999999999998</c:v>
+                  <c:v>4.3453008000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.583911111111111</c:v>
+                  <c:v>4.4534165722222223</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.7065777777777775</c:v>
+                  <c:v>4.5544159555555552</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.8212000000000002</c:v>
+                  <c:v>4.64829895</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.927777777777778</c:v>
+                  <c:v>4.7350655555555559</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.0263111111111112</c:v>
+                  <c:v>4.8147157722222218</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.1167999999999996</c:v>
+                  <c:v>4.8872496000000005</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.1992444444444441</c:v>
+                  <c:v>4.9526670388888885</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.2736444444444448</c:v>
+                  <c:v>5.0109680888888892</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.34</c:v>
+                  <c:v>5.0621527500000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.3983111111111111</c:v>
+                  <c:v>5.106221022222222</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.4485777777777784</c:v>
+                  <c:v>5.1431729055555557</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.4908000000000001</c:v>
+                  <c:v>5.1730083999999996</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.524977777777778</c:v>
+                  <c:v>5.1957275055555554</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.5511111111111111</c:v>
+                  <c:v>5.2113302222222222</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5.5692000000000004</c:v>
+                  <c:v>5.21981655</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>5.579244444444444</c:v>
+                  <c:v>5.2211864888888879</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>5.5812444444444447</c:v>
+                  <c:v>5.2154400388888895</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>5.5752000000000006</c:v>
+                  <c:v>5.2025772000000003</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5.5611111111111109</c:v>
+                  <c:v>5.1825979722222222</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>5.5389777777777782</c:v>
+                  <c:v>5.1555023555555559</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>5.5087999999999999</c:v>
+                  <c:v>5.1212903500000007</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>5.4705777777777778</c:v>
+                  <c:v>5.0799619555555555</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>5.4243111111111109</c:v>
+                  <c:v>5.0315171722222223</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>5.37</c:v>
+                  <c:v>4.975956</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>5.3076444444444437</c:v>
+                  <c:v>4.9132784388888888</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>5.2372444444444444</c:v>
+                  <c:v>4.8434844888888895</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>5.1587999999999994</c:v>
+                  <c:v>4.7665741500000003</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>5.0723111111111114</c:v>
+                  <c:v>4.682547422222223</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>4.9777777777777779</c:v>
+                  <c:v>4.5914043055555549</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>4.8752000000000004</c:v>
+                  <c:v>4.4931447999999996</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4.7645777777777774</c:v>
+                  <c:v>4.3877689055555553</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4.6459111111111113</c:v>
+                  <c:v>4.275276622222222</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>4.5191999999999997</c:v>
+                  <c:v>4.1556679499999998</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4.3844444444444441</c:v>
+                  <c:v>4.0289428888888885</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>4.2416444444444448</c:v>
+                  <c:v>3.8951014388888887</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>4.0908000000000007</c:v>
+                  <c:v>3.7541436000000004</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>3.9319111111111114</c:v>
+                  <c:v>3.6060693722222226</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>3.7649777777777782</c:v>
+                  <c:v>3.4508787555555558</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>3.59</c:v>
+                  <c:v>3.28857175</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>3.4069777777777772</c:v>
+                  <c:v>3.1191483555555553</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>3.2159111111111112</c:v>
+                  <c:v>2.9426085722222219</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>3.0167999999999995</c:v>
+                  <c:v>2.7589523999999996</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>2.8096444444444444</c:v>
+                  <c:v>2.5681798388888892</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2.5944444444444441</c:v>
+                  <c:v>2.3702908888888885</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>2.3712</c:v>
+                  <c:v>2.1652855500000001</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>2.1399111111111111</c:v>
+                  <c:v>1.9531638222222221</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>1.9005777777777781</c:v>
+                  <c:v>1.7339257055555559</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>1.6531999999999998</c:v>
+                  <c:v>1.5075711999999997</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>1.3977777777777787</c:v>
+                  <c:v>1.2741003055555562</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>1.1343111111111108</c:v>
+                  <c:v>1.033513022222222</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.8628000000000009</c:v>
+                  <c:v>0.78580935000000074</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.58324444444444445</c:v>
+                  <c:v>0.53098928888888897</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.29564444444444543</c:v>
+                  <c:v>0.26905283888888959</c:v>
                 </c:pt>
                 <c:pt idx="59">
                   <c:v>0</c:v>
@@ -612,184 +845,184 @@
             <c:numRef>
               <c:f>Sheet1!$F$2:$F$61</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
-                  <c:v>3.5642555555555551</c:v>
+                  <c:v>3.5817080177777778</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.6243555555555553</c:v>
+                  <c:v>3.6130789377777779</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.6802999999999999</c:v>
+                  <c:v>3.6412747599999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.7320888888888888</c:v>
+                  <c:v>3.6662954844444449</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.779722222222222</c:v>
+                  <c:v>3.6881411111111104</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.8231999999999999</c:v>
+                  <c:v>3.7068116400000006</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.8625222222222222</c:v>
+                  <c:v>3.722307071111111</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.8976888888888892</c:v>
+                  <c:v>3.7346274044444447</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.9286999999999996</c:v>
+                  <c:v>3.7437726399999995</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.9555555555555557</c:v>
+                  <c:v>3.7497427777777781</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.9782555555555552</c:v>
+                  <c:v>3.7525378177777782</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.9968000000000004</c:v>
+                  <c:v>3.7521577600000011</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.0111888888888885</c:v>
+                  <c:v>3.7486026044444447</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.0214222222222222</c:v>
+                  <c:v>3.7418723511111107</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4.0274999999999999</c:v>
+                  <c:v>3.731967</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.0294222222222231</c:v>
+                  <c:v>3.7188865511111118</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.0271888888888894</c:v>
+                  <c:v>3.7026310044444446</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.0207999999999995</c:v>
+                  <c:v>3.6832003599999998</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.0102555555555552</c:v>
+                  <c:v>3.6605946177777775</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.9955555555555562</c:v>
+                  <c:v>3.6348137777777785</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.9767000000000001</c:v>
+                  <c:v>3.6058578399999996</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3.9536888888888884</c:v>
+                  <c:v>3.5737268044444441</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3.9265222222222231</c:v>
+                  <c:v>3.5384206711111115</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.8952</c:v>
+                  <c:v>3.4999394399999999</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.8597222222222216</c:v>
+                  <c:v>3.4582831111111103</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.8200888888888889</c:v>
+                  <c:v>3.4134516844444445</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3.7763000000000009</c:v>
+                  <c:v>3.3654451600000002</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>3.7283555555555559</c:v>
+                  <c:v>3.3142635377777778</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>3.6762555555555556</c:v>
+                  <c:v>3.2599068177777775</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3.62</c:v>
+                  <c:v>3.202375</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3.5595888888888889</c:v>
+                  <c:v>3.1416680844444445</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.4950222222222225</c:v>
+                  <c:v>3.0777860711111114</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.4262999999999999</c:v>
+                  <c:v>3.0107289599999998</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.3534222222222225</c:v>
+                  <c:v>2.9404967511111111</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.276388888888889</c:v>
+                  <c:v>2.8670894444444444</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>3.1952000000000003</c:v>
+                  <c:v>2.79050704</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>3.1098555555555554</c:v>
+                  <c:v>2.7107495377777777</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>3.0203555555555557</c:v>
+                  <c:v>2.6278169377777783</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2.9266999999999999</c:v>
+                  <c:v>2.5417092399999994</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2.8288888888888892</c:v>
+                  <c:v>2.4524264444444448</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2.726922222222222</c:v>
+                  <c:v>2.3599685511111108</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2.6208000000000005</c:v>
+                  <c:v>2.2643355600000001</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>2.5105222222222223</c:v>
+                  <c:v>2.165527471111111</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2.3960888888888898</c:v>
+                  <c:v>2.0635442844444452</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2.2774999999999999</c:v>
+                  <c:v>1.958386</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>2.1547555555555555</c:v>
+                  <c:v>1.8500526177777774</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>2.0278555555555555</c:v>
+                  <c:v>1.7385441377777777</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1.8967999999999996</c:v>
+                  <c:v>1.6238605599999996</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1.7615888888888891</c:v>
+                  <c:v>1.5060018844444445</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1.622222222222222</c:v>
+                  <c:v>1.3849681111111107</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1.4787000000000001</c:v>
+                  <c:v>1.2607592400000001</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1.3310222222222221</c:v>
+                  <c:v>1.1333752711111109</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>1.1791888888888893</c:v>
+                  <c:v>1.0028162044444446</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>1.0231999999999999</c:v>
+                  <c:v>0.86908203999999989</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.86305555555555602</c:v>
+                  <c:v>0.73217277777777801</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.69875555555555535</c:v>
+                  <c:v>0.59208841777777754</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.53030000000000055</c:v>
+                  <c:v>0.44882896000000039</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.35768888888888883</c:v>
+                  <c:v>0.30239440444444438</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.18092222222222279</c:v>
+                  <c:v>0.15278475111111159</c:v>
                 </c:pt>
                 <c:pt idx="59">
                   <c:v>0</c:v>
@@ -812,6 +1045,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="100060928"/>
         <c:axId val="375890064"/>
@@ -1535,13 +1769,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
@@ -1891,19 +2125,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A341F2B-B38C-4DF9-AC41-594CD646DD3F}">
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="7" max="7" width="1.69140625" customWidth="1"/>
-    <col min="8" max="8" width="16.53515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.23046875" style="4"/>
+    <col min="7" max="7" width="5.3828125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="1.69140625" customWidth="1"/>
+    <col min="9" max="9" width="16.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1920,44 +2157,48 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
         <f>(ROW()-1)/60</f>
         <v>1.6666666666666666E-2</v>
       </c>
       <c r="B2" s="2">
-        <v>3.5</v>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2" s="2">
-        <v>3.62</v>
+        <v>3.202375</v>
       </c>
       <c r="E2" s="1">
         <f>4*D2*A2*(1-A2)+(B2+(C2-B2)*A2)</f>
-        <v>3.6789777777777779</v>
-      </c>
-      <c r="F2">
+        <v>3.6979761055555556</v>
+      </c>
+      <c r="F2" s="5">
         <f>(1-A2)*(1-A2)*B2+2*(1-A2)*A2*((D2-0.25*B2-0.25*C2)/0.5)+A2*A2*C2</f>
-        <v>3.5642555555555551</v>
-      </c>
-      <c r="H2" t="s">
+        <v>3.5817080177777778</v>
+      </c>
+      <c r="G2" s="1">
+        <f>IF(A2=VLOOKUP(J$8,A:A,1,TRUE),MAX(E:E),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
         <v>1</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <f>F2</f>
-        <v>3.5642555555555551</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+        <v>3.5817080177777778</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <f t="shared" ref="A3:A61" si="0">(ROW()-1)/60</f>
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="B3">
         <f>B2</f>
-        <v>3.5</v>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:D18" si="1">C2</f>
@@ -1965,32 +2206,36 @@
       </c>
       <c r="D3">
         <f t="shared" si="1"/>
-        <v>3.62</v>
+        <v>3.202375</v>
       </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E61" si="2">4*D3*A3*(1-A3)+(B3+(C3-B3)*A3)</f>
-        <v>3.8499111111111111</v>
-      </c>
-      <c r="F3">
+        <v>3.8416738222222224</v>
+      </c>
+      <c r="F3" s="5">
         <f t="shared" ref="F3:F61" si="3">(1-A3)*(1-A3)*B3+2*(1-A3)*A3*((D3-0.25*B3-0.25*C3)/0.5)+A3*A3*C3</f>
-        <v>3.6243555555555553</v>
-      </c>
-      <c r="H3" t="s">
+        <v>3.6130789377777779</v>
+      </c>
+      <c r="G3" s="1">
+        <f t="shared" ref="G3:G61" si="4">IF(A3=VLOOKUP(J$8,A:A,1,TRUE),MAX(E:E),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
         <v>5</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <f>MAX(F:F)</f>
-        <v>4.0294222222222231</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+        <v>3.7525378177777782</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B61" si="4">B3</f>
-        <v>3.5</v>
+        <f t="shared" ref="B4:B61" si="5">B3</f>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C4">
         <f t="shared" si="1"/>
@@ -1998,32 +2243,36 @@
       </c>
       <c r="D4">
         <f t="shared" si="1"/>
-        <v>3.62</v>
+        <v>3.202375</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" si="2"/>
-        <v>4.0128000000000004</v>
-      </c>
-      <c r="F4">
-        <f t="shared" si="3"/>
-        <v>3.6802999999999999</v>
-      </c>
-      <c r="H4" t="s">
+        <v>3.9782551499999999</v>
+      </c>
+      <c r="F4" s="5">
+        <f t="shared" si="3"/>
+        <v>3.6412747599999999</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
         <v>2</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <f>F61</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="B5">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
@@ -2031,25 +2280,29 @@
       </c>
       <c r="D5">
         <f t="shared" si="1"/>
-        <v>3.62</v>
+        <v>3.202375</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" si="2"/>
-        <v>4.1676444444444449</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="3"/>
-        <v>3.7320888888888888</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+        <v>4.1077200888888896</v>
+      </c>
+      <c r="F5" s="5">
+        <f t="shared" si="3"/>
+        <v>3.6662954844444449</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="B6">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
@@ -2057,31 +2310,35 @@
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
-        <v>3.62</v>
+        <v>3.202375</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="2"/>
-        <v>4.3144444444444447</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="3"/>
-        <v>3.779722222222222</v>
-      </c>
-      <c r="H6" t="s">
+        <v>4.2300686388888886</v>
+      </c>
+      <c r="F6" s="5">
+        <f t="shared" si="3"/>
+        <v>3.6881411111111104</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="2">
-        <v>-3.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J6" s="2">
+        <v>-5.5919999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="B7">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
@@ -2089,31 +2346,35 @@
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
-        <v>3.62</v>
+        <v>3.202375</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" si="2"/>
-        <v>4.4531999999999998</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="3"/>
-        <v>3.8231999999999999</v>
-      </c>
-      <c r="H7" t="s">
+        <v>4.3453008000000004</v>
+      </c>
+      <c r="F7" s="5">
+        <f t="shared" si="3"/>
+        <v>3.7068116400000006</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="2">
-        <v>6.78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J7" s="2">
+        <v>3.9940000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>0.11666666666666667</v>
       </c>
       <c r="B8">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
@@ -2121,32 +2382,36 @@
       </c>
       <c r="D8">
         <f t="shared" si="1"/>
-        <v>3.62</v>
+        <v>3.202375</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="2"/>
-        <v>4.583911111111111</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="3"/>
-        <v>3.8625222222222222</v>
-      </c>
-      <c r="H8" t="s">
+        <v>4.4534165722222223</v>
+      </c>
+      <c r="F8" s="5">
+        <f t="shared" si="3"/>
+        <v>3.722307071111111</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="1">
-        <f>ABS(I6)/ABS(I7-I6)</f>
-        <v>0.34046692607003887</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J8" s="1">
+        <f>ABS(J6)/ABS(J7-J6)</f>
+        <v>0.58335071979970787</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>0.13333333333333333</v>
       </c>
       <c r="B9">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
@@ -2154,25 +2419,29 @@
       </c>
       <c r="D9">
         <f t="shared" si="1"/>
-        <v>3.62</v>
+        <v>3.202375</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="2"/>
-        <v>4.7065777777777775</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="3"/>
-        <v>3.8976888888888892</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+        <v>4.5544159555555552</v>
+      </c>
+      <c r="F9" s="5">
+        <f t="shared" si="3"/>
+        <v>3.7346274044444447</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
       <c r="B10">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
@@ -2180,32 +2449,36 @@
       </c>
       <c r="D10">
         <f t="shared" si="1"/>
-        <v>3.62</v>
+        <v>3.202375</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="2"/>
-        <v>4.8212000000000002</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="3"/>
-        <v>3.9286999999999996</v>
-      </c>
-      <c r="H10" t="s">
+        <v>4.64829895</v>
+      </c>
+      <c r="F10" s="5">
+        <f t="shared" si="3"/>
+        <v>3.7437726399999995</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="3">
-        <f>(1-I8)*(1-I8)*B2+2*(1-I8)*I8*((D2-0.25*B2-0.25*C2)/0.5)+I8*I8*C2</f>
-        <v>3.9879937622068473</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J10" s="3">
+        <f>(1-J8)*(1-J8)*B2+2*(1-J8)*J8*((D2-0.25*B2-0.25*C2)/0.5)+J8*J8*C2</f>
+        <v>2.8670112089847457</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="B11">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
@@ -2213,32 +2486,36 @@
       </c>
       <c r="D11">
         <f t="shared" si="1"/>
-        <v>3.62</v>
+        <v>3.202375</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="2"/>
-        <v>4.927777777777778</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="3"/>
-        <v>3.9555555555555557</v>
-      </c>
-      <c r="H11" t="s">
+        <v>4.7350655555555559</v>
+      </c>
+      <c r="F11" s="5">
+        <f t="shared" si="3"/>
+        <v>3.7497427777777781</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
         <v>10</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <f>D2</f>
-        <v>3.62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+        <v>3.202375</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>0.18333333333333332</v>
       </c>
       <c r="B12">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
@@ -2246,31 +2523,35 @@
       </c>
       <c r="D12">
         <f t="shared" si="1"/>
-        <v>3.62</v>
+        <v>3.202375</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="2"/>
-        <v>5.0263111111111112</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="3"/>
-        <v>3.9782555555555552</v>
-      </c>
-      <c r="H12" t="s">
+        <v>4.8147157722222218</v>
+      </c>
+      <c r="F12" s="5">
+        <f t="shared" si="3"/>
+        <v>3.7525378177777782</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
         <v>11</v>
       </c>
-      <c r="I12" s="2">
+      <c r="J12" s="2">
         <v>2.5</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
       <c r="B13">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
@@ -2278,32 +2559,36 @@
       </c>
       <c r="D13">
         <f t="shared" si="1"/>
-        <v>3.62</v>
+        <v>3.202375</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="2"/>
-        <v>5.1167999999999996</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="3"/>
-        <v>3.9968000000000004</v>
-      </c>
-      <c r="H13" t="s">
+        <v>4.8872496000000005</v>
+      </c>
+      <c r="F13" s="5">
+        <f t="shared" si="3"/>
+        <v>3.7521577600000011</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="3">
-        <f>I11+I12-I10</f>
-        <v>2.1320062377931528</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="J13" s="3">
+        <f>J11+J12-J10</f>
+        <v>2.8353637910152543</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
         <v>0.21666666666666667</v>
       </c>
       <c r="B14">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
@@ -2311,25 +2596,29 @@
       </c>
       <c r="D14">
         <f t="shared" si="1"/>
-        <v>3.62</v>
+        <v>3.202375</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" si="2"/>
-        <v>5.1992444444444441</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="3"/>
-        <v>4.0111888888888885</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+        <v>4.9526670388888885</v>
+      </c>
+      <c r="F14" s="5">
+        <f t="shared" si="3"/>
+        <v>3.7486026044444447</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15" s="1">
         <f t="shared" si="0"/>
         <v>0.23333333333333334</v>
       </c>
       <c r="B15">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
@@ -2337,25 +2626,29 @@
       </c>
       <c r="D15">
         <f t="shared" si="1"/>
-        <v>3.62</v>
+        <v>3.202375</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" si="2"/>
-        <v>5.2736444444444448</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="3"/>
-        <v>4.0214222222222222</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+        <v>5.0109680888888892</v>
+      </c>
+      <c r="F15" s="5">
+        <f t="shared" si="3"/>
+        <v>3.7418723511111107</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
       <c r="B16">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
@@ -2363,25 +2656,29 @@
       </c>
       <c r="D16">
         <f t="shared" si="1"/>
-        <v>3.62</v>
+        <v>3.202375</v>
       </c>
       <c r="E16" s="1">
         <f t="shared" si="2"/>
-        <v>5.34</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="3"/>
-        <v>4.0274999999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+        <v>5.0621527500000001</v>
+      </c>
+      <c r="F16" s="5">
+        <f t="shared" si="3"/>
+        <v>3.731967</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="1">
         <f t="shared" si="0"/>
         <v>0.26666666666666666</v>
       </c>
       <c r="B17">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
@@ -2389,25 +2686,29 @@
       </c>
       <c r="D17">
         <f t="shared" si="1"/>
-        <v>3.62</v>
+        <v>3.202375</v>
       </c>
       <c r="E17" s="1">
         <f t="shared" si="2"/>
-        <v>5.3983111111111111</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="3"/>
-        <v>4.0294222222222231</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+        <v>5.106221022222222</v>
+      </c>
+      <c r="F17" s="5">
+        <f t="shared" si="3"/>
+        <v>3.7188865511111118</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="1">
         <f t="shared" si="0"/>
         <v>0.28333333333333333</v>
       </c>
       <c r="B18">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C18">
         <f t="shared" si="1"/>
@@ -2415,1132 +2716,1308 @@
       </c>
       <c r="D18">
         <f t="shared" si="1"/>
-        <v>3.62</v>
+        <v>3.202375</v>
       </c>
       <c r="E18" s="1">
         <f t="shared" si="2"/>
-        <v>5.4485777777777784</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="3"/>
-        <v>4.0271888888888894</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+        <v>5.1431729055555557</v>
+      </c>
+      <c r="F18" s="5">
+        <f t="shared" si="3"/>
+        <v>3.7026310044444446</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
       <c r="B19">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C19">
-        <f t="shared" ref="C19:C61" si="5">C18</f>
+        <f t="shared" ref="C19:C61" si="6">C18</f>
         <v>0</v>
       </c>
       <c r="D19">
-        <f t="shared" ref="D19:D61" si="6">D18</f>
-        <v>3.62</v>
+        <f t="shared" ref="D19:D61" si="7">D18</f>
+        <v>3.202375</v>
       </c>
       <c r="E19" s="1">
         <f t="shared" si="2"/>
-        <v>5.4908000000000001</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="3"/>
-        <v>4.0207999999999995</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+        <v>5.1730083999999996</v>
+      </c>
+      <c r="F19" s="5">
+        <f t="shared" si="3"/>
+        <v>3.6832003599999998</v>
+      </c>
+      <c r="G19" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>0.31666666666666665</v>
       </c>
       <c r="B20">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D20">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E20" s="1">
         <f t="shared" si="2"/>
-        <v>5.524977777777778</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="3"/>
-        <v>4.0102555555555552</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+        <v>5.1957275055555554</v>
+      </c>
+      <c r="F20" s="5">
+        <f t="shared" si="3"/>
+        <v>3.6605946177777775</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="B21">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D21">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E21" s="1">
         <f t="shared" si="2"/>
-        <v>5.5511111111111111</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="3"/>
-        <v>3.9955555555555562</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+        <v>5.2113302222222222</v>
+      </c>
+      <c r="F21" s="5">
+        <f t="shared" si="3"/>
+        <v>3.6348137777777785</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
         <v>0.35</v>
       </c>
       <c r="B22">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D22">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E22" s="1">
         <f t="shared" si="2"/>
-        <v>5.5692000000000004</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="3"/>
-        <v>3.9767000000000001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+        <v>5.21981655</v>
+      </c>
+      <c r="F22" s="5">
+        <f t="shared" si="3"/>
+        <v>3.6058578399999996</v>
+      </c>
+      <c r="G22" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
         <v>0.36666666666666664</v>
       </c>
       <c r="B23">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D23">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E23" s="1">
         <f t="shared" si="2"/>
-        <v>5.579244444444444</v>
-      </c>
-      <c r="F23">
-        <f t="shared" si="3"/>
-        <v>3.9536888888888884</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+        <v>5.2211864888888879</v>
+      </c>
+      <c r="F23" s="5">
+        <f t="shared" si="3"/>
+        <v>3.5737268044444441</v>
+      </c>
+      <c r="G23" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A24" s="1">
         <f t="shared" si="0"/>
         <v>0.38333333333333336</v>
       </c>
       <c r="B24">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D24">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E24" s="1">
         <f t="shared" si="2"/>
-        <v>5.5812444444444447</v>
-      </c>
-      <c r="F24">
-        <f t="shared" si="3"/>
-        <v>3.9265222222222231</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+        <v>5.2154400388888895</v>
+      </c>
+      <c r="F24" s="5">
+        <f t="shared" si="3"/>
+        <v>3.5384206711111115</v>
+      </c>
+      <c r="G24" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
       <c r="B25">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D25">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E25" s="1">
         <f t="shared" si="2"/>
-        <v>5.5752000000000006</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="3"/>
-        <v>3.8952</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+        <v>5.2025772000000003</v>
+      </c>
+      <c r="F25" s="5">
+        <f t="shared" si="3"/>
+        <v>3.4999394399999999</v>
+      </c>
+      <c r="G25" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
         <v>0.41666666666666669</v>
       </c>
       <c r="B26">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D26">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E26" s="1">
         <f t="shared" si="2"/>
-        <v>5.5611111111111109</v>
-      </c>
-      <c r="F26">
-        <f t="shared" si="3"/>
-        <v>3.8597222222222216</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+        <v>5.1825979722222222</v>
+      </c>
+      <c r="F26" s="5">
+        <f t="shared" si="3"/>
+        <v>3.4582831111111103</v>
+      </c>
+      <c r="G26" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
         <v>0.43333333333333335</v>
       </c>
       <c r="B27">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D27">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E27" s="1">
         <f t="shared" si="2"/>
-        <v>5.5389777777777782</v>
-      </c>
-      <c r="F27">
-        <f t="shared" si="3"/>
-        <v>3.8200888888888889</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
+        <v>5.1555023555555559</v>
+      </c>
+      <c r="F27" s="5">
+        <f t="shared" si="3"/>
+        <v>3.4134516844444445</v>
+      </c>
+      <c r="G27" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
         <v>0.45</v>
       </c>
       <c r="B28">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D28">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E28" s="1">
         <f t="shared" si="2"/>
-        <v>5.5087999999999999</v>
-      </c>
-      <c r="F28">
-        <f t="shared" si="3"/>
-        <v>3.7763000000000009</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+        <v>5.1212903500000007</v>
+      </c>
+      <c r="F28" s="5">
+        <f t="shared" si="3"/>
+        <v>3.3654451600000002</v>
+      </c>
+      <c r="G28" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
         <v>0.46666666666666667</v>
       </c>
       <c r="B29">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D29">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E29" s="1">
         <f t="shared" si="2"/>
-        <v>5.4705777777777778</v>
-      </c>
-      <c r="F29">
-        <f t="shared" si="3"/>
-        <v>3.7283555555555559</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+        <v>5.0799619555555555</v>
+      </c>
+      <c r="F29" s="5">
+        <f t="shared" si="3"/>
+        <v>3.3142635377777778</v>
+      </c>
+      <c r="G29" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
         <v>0.48333333333333334</v>
       </c>
       <c r="B30">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D30">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E30" s="1">
         <f t="shared" si="2"/>
-        <v>5.4243111111111109</v>
-      </c>
-      <c r="F30">
-        <f t="shared" si="3"/>
-        <v>3.6762555555555556</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+        <v>5.0315171722222223</v>
+      </c>
+      <c r="F30" s="5">
+        <f t="shared" si="3"/>
+        <v>3.2599068177777775</v>
+      </c>
+      <c r="G30" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A31" s="1">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="B31">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D31">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E31" s="1">
         <f t="shared" si="2"/>
-        <v>5.37</v>
-      </c>
-      <c r="F31">
-        <f t="shared" si="3"/>
-        <v>3.62</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
+        <v>4.975956</v>
+      </c>
+      <c r="F31" s="5">
+        <f t="shared" si="3"/>
+        <v>3.202375</v>
+      </c>
+      <c r="G31" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A32" s="1">
         <f t="shared" si="0"/>
         <v>0.51666666666666672</v>
       </c>
       <c r="B32">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D32">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E32" s="1">
         <f t="shared" si="2"/>
-        <v>5.3076444444444437</v>
-      </c>
-      <c r="F32">
-        <f t="shared" si="3"/>
-        <v>3.5595888888888889</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
+        <v>4.9132784388888888</v>
+      </c>
+      <c r="F32" s="5">
+        <f t="shared" si="3"/>
+        <v>3.1416680844444445</v>
+      </c>
+      <c r="G32" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A33" s="1">
         <f t="shared" si="0"/>
         <v>0.53333333333333333</v>
       </c>
       <c r="B33">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D33">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E33" s="1">
         <f t="shared" si="2"/>
-        <v>5.2372444444444444</v>
-      </c>
-      <c r="F33">
-        <f t="shared" si="3"/>
-        <v>3.4950222222222225</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
+        <v>4.8434844888888895</v>
+      </c>
+      <c r="F33" s="5">
+        <f t="shared" si="3"/>
+        <v>3.0777860711111114</v>
+      </c>
+      <c r="G33" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A34" s="1">
         <f t="shared" si="0"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="B34">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D34">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E34" s="1">
         <f t="shared" si="2"/>
-        <v>5.1587999999999994</v>
-      </c>
-      <c r="F34">
-        <f t="shared" si="3"/>
-        <v>3.4262999999999999</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
+        <v>4.7665741500000003</v>
+      </c>
+      <c r="F34" s="5">
+        <f t="shared" si="3"/>
+        <v>3.0107289599999998</v>
+      </c>
+      <c r="G34" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A35" s="1">
         <f t="shared" si="0"/>
         <v>0.56666666666666665</v>
       </c>
       <c r="B35">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D35">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E35" s="1">
         <f t="shared" si="2"/>
-        <v>5.0723111111111114</v>
-      </c>
-      <c r="F35">
-        <f t="shared" si="3"/>
-        <v>3.3534222222222225</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
+        <v>4.682547422222223</v>
+      </c>
+      <c r="F35" s="5">
+        <f t="shared" si="3"/>
+        <v>2.9404967511111111</v>
+      </c>
+      <c r="G35" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A36" s="1">
         <f t="shared" si="0"/>
         <v>0.58333333333333337</v>
       </c>
       <c r="B36">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D36">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E36" s="1">
         <f t="shared" si="2"/>
-        <v>4.9777777777777779</v>
-      </c>
-      <c r="F36">
-        <f t="shared" si="3"/>
-        <v>3.276388888888889</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
+        <v>4.5914043055555549</v>
+      </c>
+      <c r="F36" s="5">
+        <f t="shared" si="3"/>
+        <v>2.8670894444444444</v>
+      </c>
+      <c r="G36" s="1">
+        <f t="shared" si="4"/>
+        <v>5.2211864888888879</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A37" s="1">
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
       <c r="B37">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D37">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E37" s="1">
         <f t="shared" si="2"/>
-        <v>4.8752000000000004</v>
-      </c>
-      <c r="F37">
-        <f t="shared" si="3"/>
-        <v>3.1952000000000003</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
+        <v>4.4931447999999996</v>
+      </c>
+      <c r="F37" s="5">
+        <f t="shared" si="3"/>
+        <v>2.79050704</v>
+      </c>
+      <c r="G37" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A38" s="1">
         <f t="shared" si="0"/>
         <v>0.6166666666666667</v>
       </c>
       <c r="B38">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D38">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E38" s="1">
         <f t="shared" si="2"/>
-        <v>4.7645777777777774</v>
-      </c>
-      <c r="F38">
-        <f t="shared" si="3"/>
-        <v>3.1098555555555554</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.4">
+        <v>4.3877689055555553</v>
+      </c>
+      <c r="F38" s="5">
+        <f t="shared" si="3"/>
+        <v>2.7107495377777777</v>
+      </c>
+      <c r="G38" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A39" s="1">
         <f t="shared" si="0"/>
         <v>0.6333333333333333</v>
       </c>
       <c r="B39">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D39">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E39" s="1">
         <f t="shared" si="2"/>
-        <v>4.6459111111111113</v>
-      </c>
-      <c r="F39">
-        <f t="shared" si="3"/>
-        <v>3.0203555555555557</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.4">
+        <v>4.275276622222222</v>
+      </c>
+      <c r="F39" s="5">
+        <f t="shared" si="3"/>
+        <v>2.6278169377777783</v>
+      </c>
+      <c r="G39" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A40" s="1">
         <f t="shared" si="0"/>
         <v>0.65</v>
       </c>
       <c r="B40">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D40">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E40" s="1">
         <f t="shared" si="2"/>
-        <v>4.5191999999999997</v>
-      </c>
-      <c r="F40">
-        <f t="shared" si="3"/>
-        <v>2.9266999999999999</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.4">
+        <v>4.1556679499999998</v>
+      </c>
+      <c r="F40" s="5">
+        <f t="shared" si="3"/>
+        <v>2.5417092399999994</v>
+      </c>
+      <c r="G40" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A41" s="1">
         <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="B41">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D41">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E41" s="1">
         <f t="shared" si="2"/>
-        <v>4.3844444444444441</v>
-      </c>
-      <c r="F41">
-        <f t="shared" si="3"/>
-        <v>2.8288888888888892</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.4">
+        <v>4.0289428888888885</v>
+      </c>
+      <c r="F41" s="5">
+        <f t="shared" si="3"/>
+        <v>2.4524264444444448</v>
+      </c>
+      <c r="G41" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A42" s="1">
         <f t="shared" si="0"/>
         <v>0.68333333333333335</v>
       </c>
       <c r="B42">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D42">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E42" s="1">
         <f t="shared" si="2"/>
-        <v>4.2416444444444448</v>
-      </c>
-      <c r="F42">
-        <f t="shared" si="3"/>
-        <v>2.726922222222222</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.4">
+        <v>3.8951014388888887</v>
+      </c>
+      <c r="F42" s="5">
+        <f t="shared" si="3"/>
+        <v>2.3599685511111108</v>
+      </c>
+      <c r="G42" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A43" s="1">
         <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
       <c r="B43">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D43">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E43" s="1">
         <f t="shared" si="2"/>
-        <v>4.0908000000000007</v>
-      </c>
-      <c r="F43">
-        <f t="shared" si="3"/>
-        <v>2.6208000000000005</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.4">
+        <v>3.7541436000000004</v>
+      </c>
+      <c r="F43" s="5">
+        <f t="shared" si="3"/>
+        <v>2.2643355600000001</v>
+      </c>
+      <c r="G43" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A44" s="1">
         <f t="shared" si="0"/>
         <v>0.71666666666666667</v>
       </c>
       <c r="B44">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C44">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D44">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E44" s="1">
         <f t="shared" si="2"/>
-        <v>3.9319111111111114</v>
-      </c>
-      <c r="F44">
-        <f t="shared" si="3"/>
-        <v>2.5105222222222223</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.4">
+        <v>3.6060693722222226</v>
+      </c>
+      <c r="F44" s="5">
+        <f t="shared" si="3"/>
+        <v>2.165527471111111</v>
+      </c>
+      <c r="G44" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A45" s="1">
         <f t="shared" si="0"/>
         <v>0.73333333333333328</v>
       </c>
       <c r="B45">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C45">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D45">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E45" s="1">
         <f t="shared" si="2"/>
-        <v>3.7649777777777782</v>
-      </c>
-      <c r="F45">
-        <f t="shared" si="3"/>
-        <v>2.3960888888888898</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.4">
+        <v>3.4508787555555558</v>
+      </c>
+      <c r="F45" s="5">
+        <f t="shared" si="3"/>
+        <v>2.0635442844444452</v>
+      </c>
+      <c r="G45" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A46" s="1">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
       <c r="B46">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C46">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D46">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E46" s="1">
         <f t="shared" si="2"/>
-        <v>3.59</v>
-      </c>
-      <c r="F46">
-        <f t="shared" si="3"/>
-        <v>2.2774999999999999</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.4">
+        <v>3.28857175</v>
+      </c>
+      <c r="F46" s="5">
+        <f t="shared" si="3"/>
+        <v>1.958386</v>
+      </c>
+      <c r="G46" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A47" s="1">
         <f t="shared" si="0"/>
         <v>0.76666666666666672</v>
       </c>
       <c r="B47">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C47">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D47">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E47" s="1">
         <f t="shared" si="2"/>
-        <v>3.4069777777777772</v>
-      </c>
-      <c r="F47">
-        <f t="shared" si="3"/>
-        <v>2.1547555555555555</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.4">
+        <v>3.1191483555555553</v>
+      </c>
+      <c r="F47" s="5">
+        <f t="shared" si="3"/>
+        <v>1.8500526177777774</v>
+      </c>
+      <c r="G47" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A48" s="1">
         <f t="shared" si="0"/>
         <v>0.78333333333333333</v>
       </c>
       <c r="B48">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D48">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E48" s="1">
         <f t="shared" si="2"/>
-        <v>3.2159111111111112</v>
-      </c>
-      <c r="F48">
-        <f t="shared" si="3"/>
-        <v>2.0278555555555555</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.4">
+        <v>2.9426085722222219</v>
+      </c>
+      <c r="F48" s="5">
+        <f t="shared" si="3"/>
+        <v>1.7385441377777777</v>
+      </c>
+      <c r="G48" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A49" s="1">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
       <c r="B49">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C49">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D49">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E49" s="1">
         <f t="shared" si="2"/>
-        <v>3.0167999999999995</v>
-      </c>
-      <c r="F49">
-        <f t="shared" si="3"/>
-        <v>1.8967999999999996</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.4">
+        <v>2.7589523999999996</v>
+      </c>
+      <c r="F49" s="5">
+        <f t="shared" si="3"/>
+        <v>1.6238605599999996</v>
+      </c>
+      <c r="G49" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A50" s="1">
         <f t="shared" si="0"/>
         <v>0.81666666666666665</v>
       </c>
       <c r="B50">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D50">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E50" s="1">
         <f t="shared" si="2"/>
-        <v>2.8096444444444444</v>
-      </c>
-      <c r="F50">
-        <f t="shared" si="3"/>
-        <v>1.7615888888888891</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.4">
+        <v>2.5681798388888892</v>
+      </c>
+      <c r="F50" s="5">
+        <f t="shared" si="3"/>
+        <v>1.5060018844444445</v>
+      </c>
+      <c r="G50" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A51" s="1">
         <f t="shared" si="0"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="B51">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D51">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E51" s="1">
         <f t="shared" si="2"/>
-        <v>2.5944444444444441</v>
-      </c>
-      <c r="F51">
-        <f t="shared" si="3"/>
-        <v>1.622222222222222</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.4">
+        <v>2.3702908888888885</v>
+      </c>
+      <c r="F51" s="5">
+        <f t="shared" si="3"/>
+        <v>1.3849681111111107</v>
+      </c>
+      <c r="G51" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A52" s="1">
         <f t="shared" si="0"/>
         <v>0.85</v>
       </c>
       <c r="B52">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C52">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D52">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E52" s="1">
         <f t="shared" si="2"/>
-        <v>2.3712</v>
-      </c>
-      <c r="F52">
-        <f t="shared" si="3"/>
-        <v>1.4787000000000001</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.4">
+        <v>2.1652855500000001</v>
+      </c>
+      <c r="F52" s="5">
+        <f t="shared" si="3"/>
+        <v>1.2607592400000001</v>
+      </c>
+      <c r="G52" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A53" s="1">
         <f t="shared" si="0"/>
         <v>0.8666666666666667</v>
       </c>
       <c r="B53">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C53">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D53">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E53" s="1">
         <f t="shared" si="2"/>
-        <v>2.1399111111111111</v>
-      </c>
-      <c r="F53">
-        <f t="shared" si="3"/>
-        <v>1.3310222222222221</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.4">
+        <v>1.9531638222222221</v>
+      </c>
+      <c r="F53" s="5">
+        <f t="shared" si="3"/>
+        <v>1.1333752711111109</v>
+      </c>
+      <c r="G53" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A54" s="1">
         <f t="shared" si="0"/>
         <v>0.8833333333333333</v>
       </c>
       <c r="B54">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C54">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D54">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E54" s="1">
         <f t="shared" si="2"/>
-        <v>1.9005777777777781</v>
-      </c>
-      <c r="F54">
-        <f t="shared" si="3"/>
-        <v>1.1791888888888893</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.4">
+        <v>1.7339257055555559</v>
+      </c>
+      <c r="F54" s="5">
+        <f t="shared" si="3"/>
+        <v>1.0028162044444446</v>
+      </c>
+      <c r="G54" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A55" s="1">
         <f t="shared" si="0"/>
         <v>0.9</v>
       </c>
       <c r="B55">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D55">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E55" s="1">
         <f t="shared" si="2"/>
-        <v>1.6531999999999998</v>
-      </c>
-      <c r="F55">
-        <f t="shared" si="3"/>
-        <v>1.0231999999999999</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.4">
+        <v>1.5075711999999997</v>
+      </c>
+      <c r="F55" s="5">
+        <f t="shared" si="3"/>
+        <v>0.86908203999999989</v>
+      </c>
+      <c r="G55" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A56" s="1">
         <f t="shared" si="0"/>
         <v>0.91666666666666663</v>
       </c>
       <c r="B56">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C56">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D56">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E56" s="1">
         <f t="shared" si="2"/>
-        <v>1.3977777777777787</v>
-      </c>
-      <c r="F56">
-        <f t="shared" si="3"/>
-        <v>0.86305555555555602</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.4">
+        <v>1.2741003055555562</v>
+      </c>
+      <c r="F56" s="5">
+        <f t="shared" si="3"/>
+        <v>0.73217277777777801</v>
+      </c>
+      <c r="G56" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A57" s="1">
         <f t="shared" si="0"/>
         <v>0.93333333333333335</v>
       </c>
       <c r="B57">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C57">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D57">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E57" s="1">
         <f t="shared" si="2"/>
-        <v>1.1343111111111108</v>
-      </c>
-      <c r="F57">
-        <f t="shared" si="3"/>
-        <v>0.69875555555555535</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.4">
+        <v>1.033513022222222</v>
+      </c>
+      <c r="F57" s="5">
+        <f t="shared" si="3"/>
+        <v>0.59208841777777754</v>
+      </c>
+      <c r="G57" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A58" s="1">
         <f t="shared" si="0"/>
         <v>0.95</v>
       </c>
       <c r="B58">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C58">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D58">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E58" s="1">
         <f t="shared" si="2"/>
-        <v>0.8628000000000009</v>
-      </c>
-      <c r="F58">
-        <f t="shared" si="3"/>
-        <v>0.53030000000000055</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.4">
+        <v>0.78580935000000074</v>
+      </c>
+      <c r="F58" s="5">
+        <f t="shared" si="3"/>
+        <v>0.44882896000000039</v>
+      </c>
+      <c r="G58" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A59" s="1">
         <f t="shared" si="0"/>
         <v>0.96666666666666667</v>
       </c>
       <c r="B59">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D59">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E59" s="1">
         <f t="shared" si="2"/>
-        <v>0.58324444444444445</v>
-      </c>
-      <c r="F59">
-        <f t="shared" si="3"/>
-        <v>0.35768888888888883</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.4">
+        <v>0.53098928888888897</v>
+      </c>
+      <c r="F59" s="5">
+        <f t="shared" si="3"/>
+        <v>0.30239440444444438</v>
+      </c>
+      <c r="G59" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A60" s="1">
         <f t="shared" si="0"/>
         <v>0.98333333333333328</v>
       </c>
       <c r="B60">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C60">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D60">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E60" s="1">
         <f t="shared" si="2"/>
-        <v>0.29564444444444543</v>
-      </c>
-      <c r="F60">
-        <f t="shared" si="3"/>
-        <v>0.18092222222222279</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.4">
+        <v>0.26905283888888959</v>
+      </c>
+      <c r="F60" s="5">
+        <f t="shared" si="3"/>
+        <v>0.15278475111111159</v>
+      </c>
+      <c r="G60" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A61" s="1">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B61">
-        <f t="shared" si="4"/>
-        <v>3.5</v>
+        <f t="shared" si="5"/>
+        <v>3.5471620000000001</v>
       </c>
       <c r="C61">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D61">
-        <f t="shared" si="6"/>
-        <v>3.62</v>
+        <f t="shared" si="7"/>
+        <v>3.202375</v>
       </c>
       <c r="E61" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F61">
-        <f t="shared" si="3"/>
+      <c r="F61" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G61" s="1">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>